<commit_message>
Add lambda values for all gases 	modified:   exp11/data/fits_co2_1.nb 	modified:   exp11/data/fits_co2_2.nb 	modified:   exp11/data/fits_n_1.nb 	modified:   exp11/data/fits_n_2.nb 	modified:   exp11/data/readings.xlsx
</commit_message>
<xml_diff>
--- a/exp11/data/readings.xlsx
+++ b/exp11/data/readings.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
   <si>
     <t>PI</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Nitrogen</t>
+  </si>
+  <si>
+    <t>????</t>
   </si>
   <si>
     <t>CO2</t>
@@ -153,7 +156,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100">
-      <selection activeCell="K8" activeCellId="0" pane="topLeft" sqref="K8"/>
+      <selection activeCell="L18" activeCellId="0" pane="topLeft" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -367,6 +370,12 @@
         <f aca="false">2*$C$1*G14</f>
         <v>7.33016666666667</v>
       </c>
+      <c r="J14" s="0" t="n">
+        <v>0.489611</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
       <c r="E15" s="0" t="n">
@@ -384,6 +393,9 @@
         <f aca="false">2*$C$1*G15</f>
         <v>7.33016666666667</v>
       </c>
+      <c r="J15" s="0" t="n">
+        <v>0.230706</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="16">
       <c r="E16" s="0" t="n">
@@ -401,6 +413,17 @@
         <f aca="false">2*$C$1*G16</f>
         <v>7.33016666666667</v>
       </c>
+      <c r="I16" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <f aca="false">AVERAGE(J14:J15)</f>
+        <v>0.3601585</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <f aca="false">STDEV(J14:J15)/SQRT(2)</f>
+        <v>0.1294525</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="E17" s="0" t="n">
@@ -462,7 +485,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="22">
@@ -501,6 +524,9 @@
         <f aca="false">2*$C$1*G23</f>
         <v>7.09370967741936</v>
       </c>
+      <c r="J23" s="0" t="n">
+        <v>0.397348</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="E24" s="0" t="n">
@@ -518,6 +544,9 @@
         <f aca="false">2*$C$1*G24</f>
         <v>7.09370967741936</v>
       </c>
+      <c r="J24" s="0" t="n">
+        <v>0.354952</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="E25" s="0" t="n">
@@ -534,6 +563,17 @@
       <c r="H25" s="0" t="n">
         <f aca="false">2*$C$1*G25</f>
         <v>7.09370967741936</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <f aca="false">AVERAGE(J23:J24)</f>
+        <v>0.37615</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <f aca="false">STDEV(J23:J24)/SQRT(2)</f>
+        <v>0.021198</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="26">

</xml_diff>